<commit_message>
add support for reports grouped by organ
</commit_message>
<xml_diff>
--- a/config_portal/examples/reports.xlsx
+++ b/config_portal/examples/reports.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/tissue-data-explorer/config_portal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5E50E9-B27A-4E4C-819E-87189F7CF870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33611005-8136-4340-954B-F91F53FAD48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1360" windowWidth="27640" windowHeight="16940" xr2:uid="{F0208A07-D73A-714E-9D9A-D58D2EDDB5C8}"/>
+    <workbookView xWindow="1420" yWindow="2220" windowWidth="27740" windowHeight="18460" xr2:uid="{F0208A07-D73A-714E-9D9A-D58D2EDDB5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="reports" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -48,6 +48,18 @@
   </si>
   <si>
     <t>https://tacc.utexas.edu/</t>
+  </si>
+  <si>
+    <t>Organ ID</t>
+  </si>
+  <si>
+    <t>Organ Description</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Sphere 1</t>
   </si>
 </sst>
 </file>
@@ -438,37 +450,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749DB094-1985-CF46-B613-63CC9F1C4487}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{9E13C082-EE46-3A43-8A51-9E99116867C3}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{9E13C082-EE46-3A43-8A51-9E99116867C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor to run Docker container with a nonroot user
</commit_message>
<xml_diff>
--- a/config_portal/examples/reports.xlsx
+++ b/config_portal/examples/reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/tissue-data-explorer/config_portal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33611005-8136-4340-954B-F91F53FAD48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3604BB-3119-C74B-BE3A-7AE882D3077E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="2220" windowWidth="27740" windowHeight="18460" xr2:uid="{F0208A07-D73A-714E-9D9A-D58D2EDDB5C8}"/>
+    <workbookView xWindow="6440" yWindow="2580" windowWidth="27740" windowHeight="18460" xr2:uid="{F0208A07-D73A-714E-9D9A-D58D2EDDB5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="reports" sheetId="1" r:id="rId1"/>

</xml_diff>